<commit_message>
used scan for getting Employee.E1
</commit_message>
<xml_diff>
--- a/Dynamodb/GayatriOrganics.xlsx
+++ b/Dynamodb/GayatriOrganics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\AWS\AWS Projects\SriGayatriOrganics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\AWS\AWS Projects\SriGayatriOrganics\Dynamodb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C17A157-8CD4-46DC-A8E2-33E17782EF48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B643983F-BA79-4092-9452-429671147B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{6CF4DED7-38DB-45E0-8FA2-C6F7C28ACDF1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="3" xr2:uid="{6CF4DED7-38DB-45E0-8FA2-C6F7C28ACDF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Stores" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="135">
   <si>
     <t>Gopalapuram</t>
   </si>
@@ -289,16 +289,166 @@
   </si>
   <si>
     <t>Closing Time</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>P14</t>
+  </si>
+  <si>
+    <t>P15</t>
+  </si>
+  <si>
+    <t>P16</t>
+  </si>
+  <si>
+    <t>P17</t>
+  </si>
+  <si>
+    <t>P18</t>
+  </si>
+  <si>
+    <t>P19</t>
+  </si>
+  <si>
+    <t>P20</t>
+  </si>
+  <si>
+    <t>P21</t>
+  </si>
+  <si>
+    <t>P22</t>
+  </si>
+  <si>
+    <t>P23</t>
+  </si>
+  <si>
+    <t>P24</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>E13</t>
+  </si>
+  <si>
+    <t>E14</t>
+  </si>
+  <si>
+    <t>E15</t>
+  </si>
+  <si>
+    <t>E16</t>
+  </si>
+  <si>
+    <t>E17</t>
+  </si>
+  <si>
+    <t>E18</t>
+  </si>
+  <si>
+    <t>E19</t>
+  </si>
+  <si>
+    <t>E20</t>
+  </si>
+  <si>
+    <t>E21</t>
+  </si>
+  <si>
+    <t>E22</t>
+  </si>
+  <si>
+    <t>E23</t>
+  </si>
+  <si>
+    <t>E24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1066,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB433EAE-2CEC-4DC5-B8AB-78F4EB6EBFA7}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1098,8 +1248,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1118,8 +1268,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>88</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -1138,8 +1288,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>89</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -1158,8 +1308,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>90</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -1178,8 +1328,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>91</v>
       </c>
       <c r="B6" t="s">
         <v>35</v>
@@ -1198,8 +1348,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>6</v>
+      <c r="A7" t="s">
+        <v>92</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1218,8 +1368,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>93</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -1238,8 +1388,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
+      <c r="A9" t="s">
+        <v>94</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -1258,8 +1408,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>95</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -1278,8 +1428,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>10</v>
+      <c r="A11" t="s">
+        <v>96</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
@@ -1298,8 +1448,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>11</v>
+      <c r="A12" t="s">
+        <v>97</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
@@ -1318,8 +1468,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>12</v>
+      <c r="A13" t="s">
+        <v>98</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
@@ -1338,8 +1488,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>13</v>
+      <c r="A14" t="s">
+        <v>99</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
@@ -1358,8 +1508,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>14</v>
+      <c r="A15" t="s">
+        <v>100</v>
       </c>
       <c r="B15" t="s">
         <v>27</v>
@@ -1378,8 +1528,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>15</v>
+      <c r="A16" t="s">
+        <v>101</v>
       </c>
       <c r="B16" t="s">
         <v>28</v>
@@ -1398,8 +1548,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>16</v>
+      <c r="A17" t="s">
+        <v>102</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
@@ -1418,8 +1568,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>17</v>
+      <c r="A18" t="s">
+        <v>103</v>
       </c>
       <c r="B18" t="s">
         <v>31</v>
@@ -1438,8 +1588,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>18</v>
+      <c r="A19" t="s">
+        <v>104</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
@@ -1458,8 +1608,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>19</v>
+      <c r="A20" t="s">
+        <v>105</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
@@ -1478,8 +1628,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>20</v>
+      <c r="A21" t="s">
+        <v>106</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
@@ -1498,8 +1648,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>21</v>
+      <c r="A22" t="s">
+        <v>107</v>
       </c>
       <c r="B22" t="s">
         <v>32</v>
@@ -1518,8 +1668,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>22</v>
+      <c r="A23" t="s">
+        <v>108</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
@@ -1538,8 +1688,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>23</v>
+      <c r="A24" t="s">
+        <v>109</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
@@ -1558,8 +1708,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>24</v>
+      <c r="A25" t="s">
+        <v>110</v>
       </c>
       <c r="B25" t="s">
         <v>15</v>
@@ -1578,6 +1728,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1586,7 +1737,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA61B7F3-DB6F-41BD-A96D-CB0F5C740140}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1608,8 +1761,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>53</v>
@@ -1619,8 +1772,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>112</v>
       </c>
       <c r="B3" t="s">
         <v>54</v>
@@ -1630,8 +1783,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>113</v>
       </c>
       <c r="B4" t="s">
         <v>55</v>
@@ -1641,8 +1794,8 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>114</v>
       </c>
       <c r="B5" t="s">
         <v>56</v>
@@ -1652,8 +1805,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>115</v>
       </c>
       <c r="B6" t="s">
         <v>57</v>
@@ -1663,8 +1816,8 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>6</v>
+      <c r="A7" t="s">
+        <v>116</v>
       </c>
       <c r="B7" t="s">
         <v>58</v>
@@ -1674,8 +1827,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>117</v>
       </c>
       <c r="B8" t="s">
         <v>59</v>
@@ -1685,8 +1838,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
+      <c r="A9" t="s">
+        <v>118</v>
       </c>
       <c r="B9" t="s">
         <v>60</v>
@@ -1696,8 +1849,8 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>119</v>
       </c>
       <c r="B10" t="s">
         <v>61</v>
@@ -1707,8 +1860,8 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>10</v>
+      <c r="A11" t="s">
+        <v>120</v>
       </c>
       <c r="B11" t="s">
         <v>62</v>
@@ -1718,8 +1871,8 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>11</v>
+      <c r="A12" t="s">
+        <v>121</v>
       </c>
       <c r="B12" t="s">
         <v>63</v>
@@ -1729,8 +1882,8 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>12</v>
+      <c r="A13" t="s">
+        <v>122</v>
       </c>
       <c r="B13" t="s">
         <v>64</v>
@@ -1740,8 +1893,8 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>13</v>
+      <c r="A14" t="s">
+        <v>123</v>
       </c>
       <c r="B14" t="s">
         <v>65</v>
@@ -1751,8 +1904,8 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>14</v>
+      <c r="A15" t="s">
+        <v>124</v>
       </c>
       <c r="B15" t="s">
         <v>66</v>
@@ -1762,8 +1915,8 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>15</v>
+      <c r="A16" t="s">
+        <v>125</v>
       </c>
       <c r="B16" t="s">
         <v>67</v>
@@ -1773,8 +1926,8 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>16</v>
+      <c r="A17" t="s">
+        <v>126</v>
       </c>
       <c r="B17" t="s">
         <v>68</v>
@@ -1784,8 +1937,8 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>17</v>
+      <c r="A18" t="s">
+        <v>127</v>
       </c>
       <c r="B18" t="s">
         <v>69</v>
@@ -1795,8 +1948,8 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>18</v>
+      <c r="A19" t="s">
+        <v>128</v>
       </c>
       <c r="B19" t="s">
         <v>70</v>
@@ -1806,8 +1959,8 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>19</v>
+      <c r="A20" t="s">
+        <v>129</v>
       </c>
       <c r="B20" t="s">
         <v>71</v>
@@ -1817,8 +1970,8 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>20</v>
+      <c r="A21" t="s">
+        <v>130</v>
       </c>
       <c r="B21" t="s">
         <v>72</v>
@@ -1828,8 +1981,8 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>21</v>
+      <c r="A22" t="s">
+        <v>131</v>
       </c>
       <c r="B22" t="s">
         <v>73</v>
@@ -1839,8 +1992,8 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>22</v>
+      <c r="A23" t="s">
+        <v>132</v>
       </c>
       <c r="B23" t="s">
         <v>74</v>
@@ -1850,8 +2003,8 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>23</v>
+      <c r="A24" t="s">
+        <v>133</v>
       </c>
       <c r="B24" t="s">
         <v>75</v>
@@ -1861,8 +2014,8 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>24</v>
+      <c r="A25" t="s">
+        <v>134</v>
       </c>
       <c r="B25" t="s">
         <v>76</v>
@@ -1872,6 +2025,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rewriting the scan covering all cases
</commit_message>
<xml_diff>
--- a/Dynamodb/GayatriOrganics.xlsx
+++ b/Dynamodb/GayatriOrganics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\AWS\AWS Projects\SriGayatriOrganics\Dynamodb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B643983F-BA79-4092-9452-429671147B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A32E1BE-2D19-4443-8578-DFA3D3A1F5FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="3" xr2:uid="{6CF4DED7-38DB-45E0-8FA2-C6F7C28ACDF1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{6CF4DED7-38DB-45E0-8FA2-C6F7C28ACDF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Stores" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="111">
   <si>
     <t>Gopalapuram</t>
   </si>
@@ -361,78 +361,6 @@
   </si>
   <si>
     <t>P24</t>
-  </si>
-  <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
-    <t>E3</t>
-  </si>
-  <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>E5</t>
-  </si>
-  <si>
-    <t>E6</t>
-  </si>
-  <si>
-    <t>E7</t>
-  </si>
-  <si>
-    <t>E8</t>
-  </si>
-  <si>
-    <t>E9</t>
-  </si>
-  <si>
-    <t>E10</t>
-  </si>
-  <si>
-    <t>E11</t>
-  </si>
-  <si>
-    <t>E12</t>
-  </si>
-  <si>
-    <t>E13</t>
-  </si>
-  <si>
-    <t>E14</t>
-  </si>
-  <si>
-    <t>E15</t>
-  </si>
-  <si>
-    <t>E16</t>
-  </si>
-  <si>
-    <t>E17</t>
-  </si>
-  <si>
-    <t>E18</t>
-  </si>
-  <si>
-    <t>E19</t>
-  </si>
-  <si>
-    <t>E20</t>
-  </si>
-  <si>
-    <t>E21</t>
-  </si>
-  <si>
-    <t>E22</t>
-  </si>
-  <si>
-    <t>E23</t>
-  </si>
-  <si>
-    <t>E24</t>
   </si>
 </sst>
 </file>
@@ -976,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BDBB58E-BE00-4E67-B7D3-E2773512F21F}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1005,9 +933,6 @@
       <c r="B2" s="3">
         <v>0.875</v>
       </c>
-      <c r="C2" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
@@ -1216,7 +1141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB433EAE-2CEC-4DC5-B8AB-78F4EB6EBFA7}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -1737,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA61B7F3-DB6F-41BD-A96D-CB0F5C740140}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1761,8 +1686,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>111</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>53</v>
@@ -1772,8 +1697,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>112</v>
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>54</v>
@@ -1783,8 +1708,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>113</v>
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>55</v>
@@ -1794,8 +1719,8 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>114</v>
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>56</v>
@@ -1805,8 +1730,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>115</v>
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>57</v>
@@ -1816,8 +1741,8 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>116</v>
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>58</v>
@@ -1827,8 +1752,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>117</v>
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>59</v>
@@ -1838,8 +1763,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>118</v>
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>60</v>
@@ -1849,8 +1774,8 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>119</v>
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>61</v>
@@ -1860,8 +1785,8 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>120</v>
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>62</v>
@@ -1871,8 +1796,8 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>121</v>
+      <c r="A12">
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>63</v>
@@ -1882,8 +1807,8 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>122</v>
+      <c r="A13">
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>64</v>
@@ -1893,8 +1818,8 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>123</v>
+      <c r="A14">
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>65</v>
@@ -1904,8 +1829,8 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>124</v>
+      <c r="A15">
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>66</v>
@@ -1915,8 +1840,8 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>125</v>
+      <c r="A16">
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>67</v>
@@ -1926,8 +1851,8 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>126</v>
+      <c r="A17">
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>68</v>
@@ -1937,8 +1862,8 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>127</v>
+      <c r="A18">
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>69</v>
@@ -1948,8 +1873,8 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>128</v>
+      <c r="A19">
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>70</v>
@@ -1959,8 +1884,8 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>129</v>
+      <c r="A20">
+        <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>71</v>
@@ -1970,8 +1895,8 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>130</v>
+      <c r="A21">
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>72</v>
@@ -1981,8 +1906,8 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>131</v>
+      <c r="A22">
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>73</v>
@@ -1992,8 +1917,8 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>132</v>
+      <c r="A23">
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>74</v>
@@ -2003,8 +1928,8 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>133</v>
+      <c r="A24">
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>75</v>
@@ -2014,8 +1939,8 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>134</v>
+      <c r="A25">
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>76</v>

</xml_diff>